<commit_message>
Recent story changes in QA
</commit_message>
<xml_diff>
--- a/data/BuildingPermit/SanMateoBuildingPermits/WrongMessageRecordsSanMateo.xlsx
+++ b/data/BuildingPermit/SanMateoBuildingPermits/WrongMessageRecordsSanMateo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikjain2\SanMateo\Project\APAS_Automation_NJ\qa_automation\data\BuildingPermit\SanMateoBuildingPermits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikjain2\SanMateo\Project\pre-release\qa_automation\data\BuildingPermit\SanMateoBuildingPermits\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="105">
   <si>
     <t>CITYCODE</t>
   </si>
@@ -286,16 +286,67 @@
     <t>25/12/2019</t>
   </si>
   <si>
-    <t>ST-2018-988981</t>
-  </si>
-  <si>
-    <t>MISC-2018-988981</t>
-  </si>
-  <si>
     <t>Building Permit Starts With MISC</t>
   </si>
   <si>
     <t>Building Permit Starts With ST</t>
+  </si>
+  <si>
+    <t>BD-2018-988982</t>
+  </si>
+  <si>
+    <t>BD-2018-988983</t>
+  </si>
+  <si>
+    <t>BD-2018-988984</t>
+  </si>
+  <si>
+    <t>BD-2018-988985</t>
+  </si>
+  <si>
+    <t>BD-2018-988986</t>
+  </si>
+  <si>
+    <t>BD-2018-988987</t>
+  </si>
+  <si>
+    <t>BD-2018-988988</t>
+  </si>
+  <si>
+    <t>BD-2018-988989</t>
+  </si>
+  <si>
+    <t>BD-2018-988990</t>
+  </si>
+  <si>
+    <t>BD-2018-988991</t>
+  </si>
+  <si>
+    <t>BD-2018-988992</t>
+  </si>
+  <si>
+    <t>BD-2018-988993</t>
+  </si>
+  <si>
+    <t>BD-2018-988994</t>
+  </si>
+  <si>
+    <t>BD-2018-988995</t>
+  </si>
+  <si>
+    <t>BD-2018-988996</t>
+  </si>
+  <si>
+    <t>ST-2018-978981</t>
+  </si>
+  <si>
+    <t>MISC-2018-998981</t>
+  </si>
+  <si>
+    <t>Duplicate Record</t>
+  </si>
+  <si>
+    <t>BD-2018-108996</t>
   </si>
 </sst>
 </file>
@@ -709,9 +760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF26"/>
+  <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1434,7 +1487,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C10" s="14">
         <v>43466</v>
@@ -1508,7 +1561,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C11" s="14">
         <v>50771</v>
@@ -1582,7 +1635,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C12" s="14">
         <v>43466</v>
@@ -1656,7 +1709,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C13" s="14">
         <v>43466</v>
@@ -1730,7 +1783,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C14" s="14">
         <v>43466</v>
@@ -1804,7 +1857,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C15" s="14">
         <v>43466</v>
@@ -1878,7 +1931,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C16" s="14">
         <v>43466</v>
@@ -1950,7 +2003,7 @@
     <row r="17" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="C17" s="14">
         <v>43466</v>
@@ -2024,7 +2077,7 @@
         <v>74</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C18" s="14">
         <v>43466</v>
@@ -2098,7 +2151,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C19" s="14">
         <v>43466</v>
@@ -2172,7 +2225,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C20" s="14">
         <v>43466</v>
@@ -2246,7 +2299,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C21" s="14">
         <v>43466</v>
@@ -2320,7 +2373,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C22" s="14">
         <v>43466</v>
@@ -2394,7 +2447,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>81</v>
@@ -2468,7 +2521,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C24" s="14">
         <v>43466</v>
@@ -2542,7 +2595,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C25" s="14">
         <v>43466</v>
@@ -2593,7 +2646,7 @@
         <v>87654.6</v>
       </c>
       <c r="AA25" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AB25" s="13">
         <v>11000</v>
@@ -2616,7 +2669,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C26" s="14">
         <v>43466</v>
@@ -2667,7 +2720,7 @@
         <v>87654.6</v>
       </c>
       <c r="AA26" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB26" s="13">
         <v>11000</v>
@@ -2682,6 +2735,154 @@
         <v>43647</v>
       </c>
       <c r="AF26" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="14">
+        <v>43466</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="13">
+        <v>10</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="O27" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="S27" s="13">
+        <v>94403</v>
+      </c>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="13">
+        <v>87654.6</v>
+      </c>
+      <c r="AA27" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB27" s="13">
+        <v>11000</v>
+      </c>
+      <c r="AC27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD27" s="14">
+        <v>43658</v>
+      </c>
+      <c r="AE27" s="14">
+        <v>43647</v>
+      </c>
+      <c r="AF27" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="14">
+        <v>43466</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="13">
+        <v>10</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="S28" s="13">
+        <v>94403</v>
+      </c>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="13">
+        <v>87654.6</v>
+      </c>
+      <c r="AA28" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB28" s="13">
+        <v>11000</v>
+      </c>
+      <c r="AC28" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD28" s="14">
+        <v>43658</v>
+      </c>
+      <c r="AE28" s="14">
+        <v>43647</v>
+      </c>
+      <c r="AF28" s="13" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>